<commit_message>
Start coding xlsx-to-JSON conversion
</commit_message>
<xml_diff>
--- a/inputs/input.xlsx
+++ b/inputs/input.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinchen\Documents\ExEP_Technology_Office\Coronagraph_Roadmap_Working_Group\Error_Budget\ctr-error-budget\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A08C04-7136-47ED-A815-141EED8FCB1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0452B944-E37A-4A86-B890-A993F43C8904}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPP, no WFE" sheetId="5" r:id="rId1"/>
     <sheet name="WFE" sheetId="1" r:id="rId2"/>
     <sheet name="WFSC-PP factor" sheetId="2" r:id="rId3"/>
-    <sheet name="sensitivity coeff., ang1" sheetId="3" r:id="rId4"/>
-    <sheet name="sensitivity coeff, ang2" sheetId="4" r:id="rId5"/>
+    <sheet name="sensitivity coef, ang1" sheetId="3" r:id="rId4"/>
+    <sheet name="sensitivity coef, ang2" sheetId="4" r:id="rId5"/>
     <sheet name="Glossary" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -822,7 +822,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1782,7 +1782,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N2"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2110,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -2439,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Put off using .xlsx input; use only JSON for now
</commit_message>
<xml_diff>
--- a/inputs/input.xlsx
+++ b/inputs/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinchen\Documents\ExEP_Technology_Office\Coronagraph_Roadmap_Working_Group\Error_Budget\ctr-error-budget\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0452B944-E37A-4A86-B890-A993F43C8904}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1F6713-AB84-4493-93D4-1FB509F9B945}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPP, no WFE" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="120">
   <si>
     <t>Z2</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>Static</t>
+  </si>
+  <si>
+    <t>Spectro_1</t>
+  </si>
+  <si>
+    <t>coronagraph</t>
   </si>
 </sst>
 </file>
@@ -429,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -437,6 +443,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,44 +837,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="109.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="109.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="4"/>
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
+      <c r="C3" s="7" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -866,247 +887,337 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
+      <c r="C4" s="8">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
+      <c r="C5" s="8">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
-        <v>27</v>
+      <c r="C6" s="9">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>29</v>
+      <c r="C7" s="9">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
-        <v>31</v>
+      <c r="C8" s="8">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
+      <c r="C9" s="8">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
+      <c r="C10" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
-        <v>37</v>
+      <c r="C11" s="8">
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
-        <v>39</v>
+      <c r="C12" s="9">
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
+      <c r="C13" s="8">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
-        <v>43</v>
+      <c r="C14" s="8">
+        <v>0.02</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
         <v>54</v>
       </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="C23" s="8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
         <v>58</v>
       </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
         <v>60</v>
       </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
       </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
         <v>68</v>
       </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="C30" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="10">
+        <v>1E-10</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1E-10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
         <v>74</v>
       </c>
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="C33" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>76</v>
       </c>
       <c r="B36" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
         <v>77</v>
       </c>
-      <c r="B37" t="s">
-        <v>78</v>
+      <c r="C37" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2439,7 +2550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Draft first version of input JSON file
</commit_message>
<xml_diff>
--- a/inputs/input.xlsx
+++ b/inputs/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinchen\Documents\ExEP_Technology_Office\Coronagraph_Roadmap_Working_Group\Error_Budget\ctr-error-budget\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1F6713-AB84-4493-93D4-1FB509F9B945}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A1BCC3-50B0-48EE-A271-F990B287D105}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="sensitivity coef, ang2" sheetId="4" r:id="rId5"/>
     <sheet name="Glossary" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="128">
   <si>
     <t>Z2</t>
   </si>
@@ -242,9 +242,6 @@
     <t>core_thruput</t>
   </si>
   <si>
-    <t>Core area: area of the photometric aperture used to compute core throughput</t>
-  </si>
-  <si>
     <t>core_area</t>
   </si>
   <si>
@@ -390,6 +387,33 @@
   </si>
   <si>
     <t>coronagraph</t>
+  </si>
+  <si>
+    <t>occulter</t>
+  </si>
+  <si>
+    <t>Whether or not the system has an external occulter (i.e. starshade)</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>core_platescale_units</t>
+  </si>
+  <si>
+    <t>The angle unit to assume for core_platescale</t>
+  </si>
+  <si>
+    <t>'arcsec'</t>
+  </si>
+  <si>
+    <t>Core area: area of the photometric aperture used to compute core throughput [arcsec^2]</t>
+  </si>
+  <si>
+    <t>'contrast.csv'</t>
+  </si>
+  <si>
+    <t>'throughput.csv'</t>
   </si>
 </sst>
 </file>
@@ -435,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -452,7 +476,10 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -837,17 +864,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="109.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
@@ -865,7 +892,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -877,7 +904,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1019,7 +1046,7 @@
       </c>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1028,7 +1055,7 @@
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1037,16 +1064,16 @@
       </c>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1054,10 +1081,10 @@
         <v>52</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1068,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1076,10 +1103,10 @@
         <v>54</v>
       </c>
       <c r="C23" s="8">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1090,133 +1117,156 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
       <c r="B25" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C27" s="8">
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>63</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C28" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="C30" s="7">
+        <v>2.18E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C31" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="32" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="D30">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="C32" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" s="7">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="C34" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="10">
-        <v>1E-10</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1E-10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C37" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>75</v>
       </c>
-      <c r="B33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B35" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
         <v>76</v>
       </c>
-      <c r="B36" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="8">
+      <c r="C39" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1287,7 +1337,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1616,7 +1666,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
@@ -1945,7 +1995,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2274,7 +2324,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2566,40 +2616,40 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>85</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2608,12 +2658,12 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -2622,7 +2672,7 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2636,7 +2686,7 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2647,12 +2697,12 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2660,16 +2710,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2683,7 +2733,7 @@
         <v>1E-3</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2697,7 +2747,7 @@
         <v>0.01</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2711,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2725,7 +2775,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2736,12 +2786,12 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2749,13 +2799,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="D18" s="4"/>
     </row>
@@ -2783,37 +2833,37 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" t="s">
         <v>105</v>
-      </c>
-      <c r="B23" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
         <v>107</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>108</v>
-      </c>
-      <c r="D24" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" t="s">
         <v>110</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>111</v>
-      </c>
-      <c r="D25" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Append arrays of WFE, WFS&C, and sensitivity values to json file
</commit_message>
<xml_diff>
--- a/inputs/input.xlsx
+++ b/inputs/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinchen\Documents\ExEP_Technology_Office\Coronagraph_Roadmap_Working_Group\Error_Budget\ctr-error-budget\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A1BCC3-50B0-48EE-A271-F990B287D105}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A57D68-C784-4D15-A397-3068B2B0E3C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPP, no WFE" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="129">
   <si>
     <t>Z2</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>'throughput.csv'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5, </t>
   </si>
 </sst>
 </file>
@@ -866,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -1194,7 +1197,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -1943,7 +1946,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="B2" sqref="B2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2600,7 +2603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2824,8 +2827,8 @@
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20">
-        <v>90</v>
+      <c r="B20" t="s">
+        <v>128</v>
       </c>
       <c r="C20">
         <v>120</v>

</xml_diff>

<commit_message>
Remove temporal dimension from sensitivity array
</commit_message>
<xml_diff>
--- a/inputs/input.xlsx
+++ b/inputs/input.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinchen\Documents\ExEP_Technology_Office\Coronagraph_Roadmap_Working_Group\Error_Budget\ctr-error-budget\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A57D68-C784-4D15-A397-3068B2B0E3C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A307AE41-B583-43B7-BAF0-440E9B7B2D58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPP, no WFE" sheetId="5" r:id="rId1"/>
     <sheet name="WFE" sheetId="1" r:id="rId2"/>
     <sheet name="WFSC-PP factor" sheetId="2" r:id="rId3"/>
-    <sheet name="sensitivity coef, ang1" sheetId="3" r:id="rId4"/>
-    <sheet name="sensitivity coef, ang2" sheetId="4" r:id="rId5"/>
-    <sheet name="Glossary" sheetId="6" r:id="rId6"/>
+    <sheet name="sensitivity coef" sheetId="3" r:id="rId4"/>
+    <sheet name="Glossary" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="133">
   <si>
     <t>Z2</t>
   </si>
@@ -335,12 +334,6 @@
     <t>ANGULAR BINS</t>
   </si>
   <si>
-    <t>Min. Angular Separation [mas]</t>
-  </si>
-  <si>
-    <t>Max. Angular Separation [mas]</t>
-  </si>
-  <si>
     <t>UNITS</t>
   </si>
   <si>
@@ -416,7 +409,25 @@
     <t>'throughput.csv'</t>
   </si>
   <si>
-    <t xml:space="preserve">5, </t>
+    <t>angle 1</t>
+  </si>
+  <si>
+    <t>angle 2</t>
+  </si>
+  <si>
+    <t>angle 3</t>
+  </si>
+  <si>
+    <t>angle 5</t>
+  </si>
+  <si>
+    <t>angle 6</t>
+  </si>
+  <si>
+    <t>angle 4</t>
+  </si>
+  <si>
+    <t>User defined array in mas units</t>
   </si>
 </sst>
 </file>
@@ -873,15 +884,15 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="109.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="109.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -892,14 +903,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -907,10 +918,10 @@
         <v>21</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -921,7 +932,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -932,7 +943,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -943,7 +954,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -954,7 +965,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -965,7 +976,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -976,7 +987,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -987,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -998,7 +1009,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1009,7 +1020,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1020,7 +1031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1031,7 +1042,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1040,7 +1051,7 @@
       </c>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1049,7 +1060,7 @@
       </c>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1058,7 +1069,7 @@
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1067,16 +1078,16 @@
       </c>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1084,10 +1095,10 @@
         <v>52</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1098,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1109,7 +1120,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1120,7 +1131,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1131,18 +1142,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B26" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1153,7 +1164,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1164,18 +1175,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1186,7 +1197,7 @@
         <v>2.18E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1197,7 +1208,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -1205,21 +1216,21 @@
         <v>68</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" s="7">
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -1227,20 +1238,20 @@
         <v>71</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -1251,7 +1262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -1262,7 +1273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1291,12 +1302,12 @@
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="11.5703125"/>
+    <col min="1" max="1024" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1338,9 +1349,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1382,7 +1393,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1426,7 +1437,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1470,7 +1481,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1514,7 +1525,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1558,7 +1569,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1620,12 +1631,12 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="11.5703125"/>
+    <col min="1" max="1024" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1667,9 +1678,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
@@ -1711,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1755,7 +1766,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1799,7 +1810,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1843,7 +1854,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1887,7 +1898,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1946,15 +1957,15 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N7"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="11.5703125"/>
+    <col min="1" max="1024" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1996,9 +2007,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2040,9 +2051,9 @@
         <v>9.9999999999999994E-12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2084,9 +2095,9 @@
         <v>9.9999999999999994E-12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2128,9 +2139,9 @@
         <v>9.9999999999999994E-12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="B5" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2172,9 +2183,9 @@
         <v>9.9999999999999994E-12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="B6" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2216,9 +2227,9 @@
         <v>9.9999999999999994E-12</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="B7" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2271,358 +2282,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1024" width="11.5703125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N2" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N3" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="105" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="1025" width="11.5703125"/>
+    <col min="5" max="10" width="11.88671875" customWidth="1"/>
+    <col min="11" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>79</v>
       </c>
@@ -2636,12 +2318,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
         <v>84</v>
@@ -2650,7 +2332,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2664,7 +2346,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -2678,7 +2360,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2692,7 +2374,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2703,7 +2385,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>92</v>
       </c>
@@ -2711,7 +2393,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>79</v>
       </c>
@@ -2725,7 +2407,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2739,7 +2421,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2753,7 +2435,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2767,7 +2449,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2781,7 +2463,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2792,81 +2474,55 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="D17" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="4" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>60</v>
-      </c>
-      <c r="C19">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>104</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="D24" t="s">
         <v>106</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>107</v>
       </c>
-      <c r="D24" t="s">
+      <c r="B25" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D25" t="s">
         <v>109</v>
-      </c>
-      <c r="B25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D25" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write EXOSIMS JSON file with updated ppFact
</commit_message>
<xml_diff>
--- a/inputs/input.xlsx
+++ b/inputs/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinchen\Documents\ExEP_Technology_Office\Coronagraph_Roadmap_Working_Group\Error_Budget\ctr-error-budget\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A307AE41-B583-43B7-BAF0-440E9B7B2D58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F642CDEC-958D-4F0A-9086-98119D78D386}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPP, no WFE" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="130">
   <si>
     <t>Z2</t>
   </si>
@@ -355,9 +355,6 @@
     <t>Sensitivity Coefficients</t>
   </si>
   <si>
-    <t>1/pm</t>
-  </si>
-  <si>
     <t>change in contrast per change in WFE</t>
   </si>
   <si>
@@ -418,16 +415,10 @@
     <t>angle 3</t>
   </si>
   <si>
-    <t>angle 5</t>
-  </si>
-  <si>
-    <t>angle 6</t>
-  </si>
-  <si>
-    <t>angle 4</t>
-  </si>
-  <si>
     <t>User defined array in mas units</t>
+  </si>
+  <si>
+    <t>ppt/pm</t>
   </si>
 </sst>
 </file>
@@ -880,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -906,7 +897,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -918,7 +909,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,7 +1074,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="7"/>
     </row>
@@ -1095,7 +1086,7 @@
         <v>52</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,13 +1135,13 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
         <v>117</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,13 +1168,13 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" t="s">
         <v>120</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1216,7 +1207,7 @@
         <v>68</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,7 +1215,7 @@
         <v>70</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="7">
         <v>1.2999999999999999E-3</v>
@@ -1238,7 +1229,7 @@
         <v>71</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1"/>
     </row>
@@ -1247,7 +1238,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" s="7"/>
     </row>
@@ -1299,7 +1290,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1342,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -1680,7 +1671,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
@@ -1954,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2009,7 +2000,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2053,7 +2044,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2097,7 +2088,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1">
         <v>9.9999999999999994E-12</v>
@@ -2136,138 +2127,6 @@
         <v>9.9999999999999994E-12</v>
       </c>
       <c r="N4" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N5" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N6" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="C7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="E7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="F7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="G7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="H7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="I7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="J7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="K7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="L7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="M7" s="1">
-        <v>9.9999999999999994E-12</v>
-      </c>
-      <c r="N7" s="1">
         <v>9.9999999999999994E-12</v>
       </c>
     </row>
@@ -2286,7 +2145,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2323,7 +2182,7 @@
         <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
         <v>84</v>
@@ -2481,7 +2340,7 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2519,10 +2378,10 @@
         <v>107</v>
       </c>
       <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" t="s">
         <v>108</v>
-      </c>
-      <c r="D25" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>